<commit_message>
add factory for remote service promotion
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/promotion/RemoteServicePromotionTestData.xlsx
+++ b/src/test/java/remoteService/promotion/RemoteServicePromotionTestData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinwinarko/eclipse-workspace/DanaPulsaAutomationTest/src/test/java/testCases/otp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/promotion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2CB71B-339A-0640-8948-D1CA482813D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCB7090-6EDA-F14B-803B-42C6EACCC62D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Get Promotion Vouchers" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,27 +33,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
-    <t>id</t>
+    <t>user id</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>9999</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,12 +67,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -98,25 +105,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -429,64 +431,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09F2C92-1070-F549-ABD8-21E67EECDFEF}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update get voucher details code
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/promotion/RemoteServicePromotionTestData.xlsx
+++ b/src/test/java/remoteService/promotion/RemoteServicePromotionTestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/promotion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCB7090-6EDA-F14B-803B-42C6EACCC62D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D40C10-A012-E24F-8EAB-BACCA3335671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" activeTab="1" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Get Promotion Vouchers" sheetId="2" r:id="rId1"/>
+    <sheet name="Get Voucher Details" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>user id</t>
   </si>
@@ -45,6 +46,27 @@
   </si>
   <si>
     <t>9999</t>
+  </si>
+  <si>
+    <t>voucher id</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Valid ID</t>
+  </si>
+  <si>
+    <t>Undefined ID</t>
+  </si>
+  <si>
+    <t>Empty String</t>
   </si>
 </sst>
 </file>
@@ -108,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -117,6 +139,18 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09F2C92-1070-F549-ABD8-21E67EECDFEF}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,4 +525,60 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F7BCED6-A6C1-F744-AE33-9620C5267380}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update get my vouchers code
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/promotion/RemoteServicePromotionTestData.xlsx
+++ b/src/test/java/remoteService/promotion/RemoteServicePromotionTestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/promotion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D40C10-A012-E24F-8EAB-BACCA3335671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60DE416-600A-E641-B214-D001D0306E02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" activeTab="1" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Get Promotion Vouchers" sheetId="2" r:id="rId1"/>
-    <sheet name="Get Voucher Details" sheetId="3" r:id="rId2"/>
+    <sheet name="Get My Vouchers" sheetId="4" r:id="rId2"/>
+    <sheet name="Get Voucher Details" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
-  <si>
-    <t>user id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
   <si>
     <t>page</t>
   </si>
@@ -67,6 +65,24 @@
   </si>
   <si>
     <t>Empty String</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>Valid user id and page</t>
+  </si>
+  <si>
+    <t>Undefined user id</t>
+  </si>
+  <si>
+    <t>Undefined page</t>
+  </si>
+  <si>
+    <t>Empty string page</t>
+  </si>
+  <si>
+    <t>Empty string user id</t>
   </si>
 </sst>
 </file>
@@ -130,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -149,6 +165,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -465,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09F2C92-1070-F549-ABD8-21E67EECDFEF}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,49 +497,67 @@
     <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
         <v>9999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -528,11 +565,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63BD89A-7FF1-DD43-8183-237CABA760D5}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F7BCED6-A6C1-F744-AE33-9620C5267380}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,39 +659,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="6"/>
     </row>

</xml_diff>